<commit_message>
Add openai model parameters and prompts data
</commit_message>
<xml_diff>
--- a/chat_prompts.xlsx
+++ b/chat_prompts.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troyzada/VSCode/llm-and-misinformation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21A611F-EE88-3944-B21B-F0BE1441E608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAB4720-D07B-DD45-BC2E-B3A08978441A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2733,10 +2733,10 @@
 (F) S1 radiculopathy</t>
   </si>
   <si>
-    <t>usmle_1_a</t>
-  </si>
-  <si>
-    <t>usmle_2_a</t>
+    <t>usmle_1_a_0</t>
+  </si>
+  <si>
+    <t>usmle_2_a_0</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added sentence drop experiment to prompt GPT-4
</commit_message>
<xml_diff>
--- a/chat_prompts.xlsx
+++ b/chat_prompts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/troyzada/VSCode/llm-and-misinformation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAB4720-D07B-DD45-BC2E-B3A08978441A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CF5D4-CB43-B743-BD05-EAF3DCE2E705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33140" yWindow="-6100" windowWidth="29400" windowHeight="17120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="263">
   <si>
     <t>usmle_1_q_num</t>
   </si>
@@ -2737,6 +2737,120 @@
   </si>
   <si>
     <t>usmle_2_a_0</t>
+  </si>
+  <si>
+    <t>ne_match</t>
+  </si>
+  <si>
+    <t>ex_match</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>AIPC</t>
+  </si>
+  <si>
+    <t>IIPC</t>
+  </si>
+  <si>
+    <t>CPCA</t>
+  </si>
+  <si>
+    <t>PCIA</t>
+  </si>
+  <si>
+    <t>CPCPC</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>CIC</t>
+  </si>
+  <si>
+    <t>PCPCI</t>
+  </si>
+  <si>
+    <t>PCCC</t>
+  </si>
+  <si>
+    <t>ICC</t>
+  </si>
+  <si>
+    <t>PCAC</t>
+  </si>
+  <si>
+    <t>IPCI</t>
+  </si>
+  <si>
+    <t>AII</t>
+  </si>
+  <si>
+    <t>PCPCPC</t>
+  </si>
+  <si>
+    <t>PCII</t>
+  </si>
+  <si>
+    <t>CII</t>
+  </si>
+  <si>
+    <t>CPCC</t>
+  </si>
+  <si>
+    <t>CCPC</t>
+  </si>
+  <si>
+    <t>CAPC</t>
+  </si>
+  <si>
+    <t>PCIPC</t>
+  </si>
+  <si>
+    <t>IIC</t>
+  </si>
+  <si>
+    <t>IIA</t>
+  </si>
+  <si>
+    <t>IAI</t>
+  </si>
+  <si>
+    <t>IPCC</t>
+  </si>
+  <si>
+    <t>PCAPC</t>
+  </si>
+  <si>
+    <t>CIPC</t>
+  </si>
+  <si>
+    <t>CCI</t>
+  </si>
+  <si>
+    <t>PCPCC</t>
+  </si>
+  <si>
+    <t>IPCPC</t>
+  </si>
+  <si>
+    <t>PCCPC</t>
+  </si>
+  <si>
+    <t>CPCI</t>
+  </si>
+  <si>
+    <t>ACPC</t>
+  </si>
+  <si>
+    <t>ICPC</t>
+  </si>
+  <si>
+    <t>PCIC</t>
   </si>
 </sst>
 </file>
@@ -3124,10 +3238,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ALT110"/>
+  <dimension ref="A1:ALV110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L95" sqref="L95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3135,11 +3249,13 @@
     <col min="1" max="1" width="13" style="1" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" style="2" customWidth="1"/>
     <col min="3" max="11" width="8.33203125" style="1"/>
-    <col min="13" max="13" width="48.5" style="1" customWidth="1"/>
-    <col min="14" max="1008" width="8.33203125" style="1"/>
+    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="1"/>
+    <col min="15" max="15" width="48.5" style="1" customWidth="1"/>
+    <col min="16" max="1010" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3173,1473 +3289,2043 @@
       <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2.1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="N3">
         <v>2.1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="340" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3.1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="N4">
         <v>3.1</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4.0999999999999996</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N5">
         <v>4.0999999999999996</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="340" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="340" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5.0999999999999996</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6.1</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="N7">
         <v>6.1</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="306" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="306" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>8.1</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N8">
         <v>7.1</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>9.1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N9">
         <v>8.1</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="323" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>10.1</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="N10">
         <v>9.1</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>12.1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N11">
         <v>10.1</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>13.1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="N12">
         <v>11.1</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>14.1</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N13">
         <v>12.1</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>15.1</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="N14">
         <v>13.1</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="323" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="323" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>16.100000000000001</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="N15">
         <v>14.1</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>17.100000000000001</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N16">
         <v>15.1</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>19.100000000000001</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N17">
         <v>16.100000000000001</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" ht="306" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>20.100000000000001</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N18">
         <v>17.100000000000001</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>22.1</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N19">
         <v>18.100000000000001</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="372" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>23.1</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="N20">
         <v>19.100000000000001</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>24.1</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N21">
         <v>20.100000000000001</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>25.1</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N22">
         <v>21.1</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>26.1</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="N23">
         <v>22.1</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>27.1</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N24">
         <v>23.1</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>28.1</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N25">
         <v>24.1</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>29.1</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N26">
         <v>27.1</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>31.1</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N27">
         <v>28.1</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>33.1</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N28">
         <v>29.1</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>35.1</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N29">
         <v>30.1</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>37.1</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N30">
         <v>31.1</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" ht="372" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>38.1</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="N31">
         <v>32.1</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="388" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>39.1</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N32">
         <v>34.1</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>41.1</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N33">
         <v>35.1</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43.1</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N34">
         <v>36.1</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="O34" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" ht="372" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>45.1</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="N35">
         <v>37.1</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>46.1</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N36">
         <v>38.1</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="O36" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>48.1</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N37">
         <v>39.1</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="O37" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>49.1</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N38">
         <v>40.1</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>50.1</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="N39">
         <v>41.1</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>51.1</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N40">
         <v>42.1</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>52.1</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N41">
         <v>43.1</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>54.1</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N42">
         <v>44.1</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>55.1</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N43">
         <v>45.1</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" ht="372" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>57.1</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="N44">
         <v>46.1</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>58.1</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N45">
         <v>47.1</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="O45" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>59.1</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N46">
         <v>48.1</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="O46" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>60.1</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N47">
         <v>49.1</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="O47" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>61.1</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="N48">
         <v>50.1</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="O48" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>63.1</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="L49">
+      <c r="L49" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N49">
         <v>51.1</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="O49" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>64.099999999999994</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="L50">
+      <c r="L50" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M50" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="N50">
         <v>52.1</v>
       </c>
-      <c r="M50" s="1" t="s">
+      <c r="O50" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>65.099999999999994</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="L51">
+      <c r="L51" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N51">
         <v>55.1</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="O51" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>66.099999999999994</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N52">
         <v>56.1</v>
       </c>
-      <c r="M52" s="1" t="s">
+      <c r="O52" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>67.099999999999994</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="N53">
         <v>57.1</v>
       </c>
-      <c r="M53" s="1" t="s">
+      <c r="O53" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>69.099999999999994</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="L54">
+      <c r="L54" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N54">
         <v>58.1</v>
       </c>
-      <c r="M54" s="1" t="s">
+      <c r="O54" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>70.099999999999994</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="L55">
+      <c r="L55" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N55">
         <v>59.1</v>
       </c>
-      <c r="M55" s="1" t="s">
+      <c r="O55" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>71.099999999999994</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="L56">
+      <c r="L56" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N56">
         <v>61.1</v>
       </c>
-      <c r="M56" s="1" t="s">
+      <c r="O56" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="340" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>72.099999999999994</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="L57">
+      <c r="L57" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N57">
         <v>62.1</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="O57" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" ht="388" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>73.099999999999994</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="L58">
+      <c r="L58" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N58">
         <v>63.1</v>
       </c>
-      <c r="M58" s="1" t="s">
+      <c r="O58" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>74.099999999999994</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="L59">
+      <c r="L59" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N59">
         <v>64.099999999999994</v>
       </c>
-      <c r="M59" s="1" t="s">
+      <c r="O59" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>75.099999999999994</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="L60">
+      <c r="L60" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N60">
         <v>65.099999999999994</v>
       </c>
-      <c r="M60" s="1" t="s">
+      <c r="O60" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>76.099999999999994</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L61">
+      <c r="L61" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N61">
         <v>66.099999999999994</v>
       </c>
-      <c r="M61" s="1" t="s">
+      <c r="O61" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>78.099999999999994</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="L62">
+      <c r="L62" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N62">
         <v>67.099999999999994</v>
       </c>
-      <c r="M62" s="1" t="s">
+      <c r="O62" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>79.099999999999994</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="L63">
+      <c r="L63" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="N63">
         <v>68.099999999999994</v>
       </c>
-      <c r="M63" s="1" t="s">
+      <c r="O63" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>81.099999999999994</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="L64">
+      <c r="L64" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="N64">
         <v>69.099999999999994</v>
       </c>
-      <c r="M64" s="1" t="s">
+      <c r="O64" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" ht="372" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>82.1</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N65">
         <v>70.099999999999994</v>
       </c>
-      <c r="M65" s="1" t="s">
+      <c r="O65" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>83.1</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="L66">
+      <c r="L66" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="N66">
         <v>71.099999999999994</v>
       </c>
-      <c r="M66" s="1" t="s">
+      <c r="O66" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>84.1</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N67">
         <v>72.099999999999994</v>
       </c>
-      <c r="M67" s="1" t="s">
+      <c r="O67" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>86.1</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="L68">
+      <c r="L68" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="N68">
         <v>73.099999999999994</v>
       </c>
-      <c r="M68" s="1" t="s">
+      <c r="O68" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="289" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" ht="289" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>87.1</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L69">
+      <c r="L69" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N69">
         <v>74.099999999999994</v>
       </c>
-      <c r="M69" s="1" t="s">
+      <c r="O69" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>90.1</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="L70">
+      <c r="L70" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N70">
         <v>75.099999999999994</v>
       </c>
-      <c r="M70" s="1" t="s">
+      <c r="O70" s="1" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>91.1</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="L71">
+      <c r="L71" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N71">
         <v>77.099999999999994</v>
       </c>
-      <c r="M71" s="1" t="s">
+      <c r="O71" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>92.1</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N72">
         <v>78.099999999999994</v>
       </c>
-      <c r="M72" s="1" t="s">
+      <c r="O72" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>93.1</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="L73">
+      <c r="L73" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N73">
         <v>79.099999999999994</v>
       </c>
-      <c r="M73" s="1" t="s">
+      <c r="O73" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>94.1</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="L74">
+      <c r="L74" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N74">
         <v>81.099999999999994</v>
       </c>
-      <c r="M74" s="1" t="s">
+      <c r="O74" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>95.1</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="L75">
+      <c r="L75" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="N75">
         <v>82.1</v>
       </c>
-      <c r="M75" s="1" t="s">
+      <c r="O75" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>96.1</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="L76">
+      <c r="L76" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N76">
         <v>83.1</v>
       </c>
-      <c r="M76" s="1" t="s">
+      <c r="O76" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" ht="323" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>97.1</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="L77">
+      <c r="L77" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N77">
         <v>84.1</v>
       </c>
-      <c r="M77" s="1" t="s">
+      <c r="O77" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>98.1</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="L78">
+      <c r="L78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N78">
         <v>85.1</v>
       </c>
-      <c r="M78" s="1" t="s">
+      <c r="O78" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>99.1</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="L79">
+      <c r="L79" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="N79">
         <v>86.1</v>
       </c>
-      <c r="M79" s="1" t="s">
+      <c r="O79" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>101.1</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N80">
         <v>88.1</v>
       </c>
-      <c r="M80" s="1" t="s">
+      <c r="O80" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>102.1</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="L81">
+      <c r="L81" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N81">
         <v>89.1</v>
       </c>
-      <c r="M81" s="1" t="s">
+      <c r="O81" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>103.1</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="L82">
+      <c r="L82" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N82">
         <v>90.1</v>
       </c>
-      <c r="M82" s="1" t="s">
+      <c r="O82" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>104.1</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="L83">
+      <c r="L83" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N83">
         <v>91.1</v>
       </c>
-      <c r="M83" s="1" t="s">
+      <c r="O83" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>106.1</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="L84">
+      <c r="L84" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="N84">
         <v>92.1</v>
       </c>
-      <c r="M84" s="1" t="s">
+      <c r="O84" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>107.1</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="L85">
+      <c r="L85" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N85">
         <v>93.1</v>
       </c>
-      <c r="M85" s="1" t="s">
+      <c r="O85" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>108.1</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="L86">
+      <c r="L86" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N86">
         <v>94.1</v>
       </c>
-      <c r="M86" s="1" t="s">
+      <c r="O86" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>109.1</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="L87">
+      <c r="L87" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="N87">
         <v>95.1</v>
       </c>
-      <c r="M87" s="1" t="s">
+      <c r="O87" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>110.1</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="L88">
+      <c r="L88" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="N88">
         <v>96.1</v>
       </c>
-      <c r="M88" s="1" t="s">
+      <c r="O88" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>111.1</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="L89">
+      <c r="L89" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="N89">
         <v>97.1</v>
       </c>
-      <c r="M89" s="1" t="s">
+      <c r="O89" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="340" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" ht="340" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>112.1</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="L90">
+      <c r="L90" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N90">
         <v>98.1</v>
       </c>
-      <c r="M90" s="1" t="s">
+      <c r="O90" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" ht="388" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>115.1</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="L91">
+      <c r="L91" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="N91">
         <v>99.1</v>
       </c>
-      <c r="M91" s="1" t="s">
+      <c r="O91" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>116.1</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="L92">
+      <c r="L92" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="N92">
         <v>100.1</v>
       </c>
-      <c r="M92" s="1" t="s">
+      <c r="O92" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>117.1</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="L93">
+      <c r="L93" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N93">
         <v>101.1</v>
       </c>
-      <c r="M93" s="1" t="s">
+      <c r="O93" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" ht="404" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>118.1</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="L94">
+      <c r="L94" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="N94">
         <v>102.1</v>
       </c>
-      <c r="M94" s="1" t="s">
+      <c r="O94" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>119.1</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="L95">
+      <c r="L95" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="N95">
         <v>103.1</v>
       </c>
-      <c r="M95" s="1" t="s">
+      <c r="O95" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L96">
+    <row r="96" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N96">
         <v>104.1</v>
       </c>
-      <c r="M96" s="1" t="s">
+      <c r="O96" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="97" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L97">
+    <row r="97" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N97">
         <v>105.1</v>
       </c>
-      <c r="M97" s="1" t="s">
+      <c r="O97" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L98">
+    <row r="98" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N98">
         <v>106.1</v>
       </c>
-      <c r="M98" s="1" t="s">
+      <c r="O98" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="99" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L99">
+    <row r="99" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N99">
         <v>108.1</v>
       </c>
-      <c r="M99" s="1" t="s">
+      <c r="O99" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L100">
+    <row r="100" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N100">
         <v>109.1</v>
       </c>
-      <c r="M100" s="1" t="s">
+      <c r="O100" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="12:13" ht="272" x14ac:dyDescent="0.2">
-      <c r="L101">
+    <row r="101" spans="14:15" ht="272" x14ac:dyDescent="0.2">
+      <c r="N101">
         <v>110.1</v>
       </c>
-      <c r="M101" s="1" t="s">
+      <c r="O101" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="102" spans="12:13" ht="289" x14ac:dyDescent="0.2">
-      <c r="L102">
+    <row r="102" spans="14:15" ht="289" x14ac:dyDescent="0.2">
+      <c r="N102">
         <v>111.1</v>
       </c>
-      <c r="M102" s="1" t="s">
+      <c r="O102" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="12:13" ht="356" x14ac:dyDescent="0.2">
-      <c r="L103">
+    <row r="103" spans="14:15" ht="356" x14ac:dyDescent="0.2">
+      <c r="N103">
         <v>112.1</v>
       </c>
-      <c r="M103" s="1" t="s">
+      <c r="O103" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="104" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L104">
+    <row r="104" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N104">
         <v>113.1</v>
       </c>
-      <c r="M104" s="1" t="s">
+      <c r="O104" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="105" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L105">
+    <row r="105" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N105">
         <v>115.1</v>
       </c>
-      <c r="M105" s="1" t="s">
+      <c r="O105" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="106" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L106">
+    <row r="106" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N106">
         <v>116.1</v>
       </c>
-      <c r="M106" s="1" t="s">
+      <c r="O106" s="1" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="107" spans="12:13" ht="323" x14ac:dyDescent="0.2">
-      <c r="L107">
+    <row r="107" spans="14:15" ht="323" x14ac:dyDescent="0.2">
+      <c r="N107">
         <v>117.1</v>
       </c>
-      <c r="M107" s="1" t="s">
+      <c r="O107" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="108" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L108">
+    <row r="108" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N108">
         <v>118.1</v>
       </c>
-      <c r="M108" s="1" t="s">
+      <c r="O108" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="109" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L109">
+    <row r="109" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N109">
         <v>119.1</v>
       </c>
-      <c r="M109" s="1" t="s">
+      <c r="O109" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="110" spans="12:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="L110">
+    <row r="110" spans="14:15" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="N110">
         <v>120.1</v>
       </c>
-      <c r="M110" s="1" t="s">
+      <c r="O110" s="1" t="s">
         <v>222</v>
       </c>
     </row>

</xml_diff>